<commit_message>
Started adding the OD to the report
</commit_message>
<xml_diff>
--- a/data/Object Dictionary.xlsx
+++ b/data/Object Dictionary.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25125" windowHeight="12435" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="WIFI 0x1" sheetId="1" r:id="rId1"/>
     <sheet name="IMU 0x3" sheetId="2" r:id="rId2"/>
     <sheet name="Sevcon 0x7" sheetId="3" r:id="rId3"/>
-    <sheet name="GPS 0x14" sheetId="4" r:id="rId4"/>
+    <sheet name="GPS 0xD" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
   <si>
     <t>Message Type (binary)</t>
   </si>
@@ -330,13 +331,109 @@
   </si>
   <si>
     <t>Dwork</t>
+  </si>
+  <si>
+    <t>Scaling</t>
+  </si>
+  <si>
+    <t>Fields</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Wifi 0001</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>0x00 = Config</t>
+  </si>
+  <si>
+    <t>0x01 = Start</t>
+  </si>
+  <si>
+    <t>0x02 = Stop</t>
+  </si>
+  <si>
+    <t>IMU 0010</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Pressure, Temperature</t>
+  </si>
+  <si>
+    <t>1, 1</t>
+  </si>
+  <si>
+    <t>kPa, degC</t>
+  </si>
+  <si>
+    <t>Ax, Ay, Az</t>
+  </si>
+  <si>
+    <t>0.00478</t>
+  </si>
+  <si>
+    <t>\si{\meter \per \second \squared}</t>
+  </si>
+  <si>
+    <t>Gx, Gy, Gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.000266 </t>
+  </si>
+  <si>
+    <t>rad/s</t>
+  </si>
+  <si>
+    <t>Mx, My, Mz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.15 </t>
+  </si>
+  <si>
+    <t>\si{\micro \tesla}</t>
+  </si>
+  <si>
+    <t>Ax, Ay, Az, Gx</t>
+  </si>
+  <si>
+    <t>0.00478,  0.000266</t>
+  </si>
+  <si>
+    <t>\si{\meter \per \second \squared}, rad/s</t>
+  </si>
+  <si>
+    <t>Gy, Gz, Mx, My</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0.000266, 0.15</t>
+  </si>
+  <si>
+    <t>rad/s, \si{\micro \tesla}</t>
+  </si>
+  <si>
+    <t>Mz, Yaw, Pitch, Roll</t>
+  </si>
+  <si>
+    <t>0.15, 1e-4</t>
+  </si>
+  <si>
+    <t>\si{\micro \tesla}, degree</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -344,13 +441,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -365,7 +476,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -390,10 +501,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -677,8 +791,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -807,7 +921,7 @@
   <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,12 +966,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1106,7 @@
         <v>53</v>
       </c>
       <c r="K7" s="8"/>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="10" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1016,7 +1130,7 @@
         <v>57</v>
       </c>
       <c r="K8" s="8"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
@@ -1038,7 +1152,7 @@
         <v>60</v>
       </c>
       <c r="K9" s="8"/>
-      <c r="L9" s="9"/>
+      <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -1075,6 +1189,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="L7:L9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="F9:G9"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="H8:I8"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="D5:E5"/>
     <mergeCell ref="F5:G5"/>
     <mergeCell ref="H5:I5"/>
@@ -1085,22 +1215,6 @@
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="H4:I4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="L7:L9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="F9:G9"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="H8:I8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1111,7 +1225,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="F30:G30"/>
+      <selection activeCell="M14" sqref="M14:P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1156,12 +1270,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -1372,22 +1486,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1442,12 +1556,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -1462,18 +1576,18 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="10" t="s">
+      <c r="D3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="L3" t="s">
         <v>13</v>
       </c>
@@ -1488,12 +1602,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
+      <c r="G4" s="9"/>
       <c r="L4" t="s">
         <v>16</v>
       </c>
@@ -1508,4 +1622,273 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3">
+        <v>4</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="3">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9" s="3">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>6</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="3">
+        <v>6</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="5"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="5"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="F15" t="s">
+        <v>132</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
finished OD, wrote some about power requirements
</commit_message>
<xml_diff>
--- a/data/Object Dictionary.xlsx
+++ b/data/Object Dictionary.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="151">
   <si>
     <t>Message Type (binary)</t>
   </si>
@@ -427,6 +427,60 @@
   </si>
   <si>
     <t>\si{\micro \tesla}, degree</t>
+  </si>
+  <si>
+    <t>Sevcon 0100</t>
+  </si>
+  <si>
+    <t>Id,Iq,Vd,Vq</t>
+  </si>
+  <si>
+    <t>0.0625</t>
+  </si>
+  <si>
+    <t>I_a, I_b, I_c, \Omega_e</t>
+  </si>
+  <si>
+    <t>0.0625, 1e-4</t>
+  </si>
+  <si>
+    <t>A, rad</t>
+  </si>
+  <si>
+    <t>A,V</t>
+  </si>
+  <si>
+    <t>V_a, V_b, V_c, \Omega_e</t>
+  </si>
+  <si>
+    <t>V, rad</t>
+  </si>
+  <si>
+    <t>Speed, Torque</t>
+  </si>
+  <si>
+    <t>\frac{km}{h}, Nm</t>
+  </si>
+  <si>
+    <t>GPS 1110</t>
+  </si>
+  <si>
+    <t>Lattitude, Longitude</t>
+  </si>
+  <si>
+    <t>deg (first bit indicates south, west respectivel)</t>
+  </si>
+  <si>
+    <t>Altitude</t>
+  </si>
+  <si>
+    <t>s32</t>
+  </si>
+  <si>
+    <t>0.1</t>
+  </si>
+  <si>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -476,7 +530,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
@@ -497,18 +551,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -807,16 +862,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
@@ -880,15 +935,15 @@
       <c r="D19" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="8" t="s">
+      <c r="E19" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="8"/>
-      <c r="I19" s="8"/>
-      <c r="J19" s="8"/>
-      <c r="K19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
       <c r="L19" t="s">
         <v>46</v>
       </c>
@@ -942,16 +997,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
@@ -966,12 +1021,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -986,18 +1041,18 @@
       <c r="C3" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
       <c r="L3" t="s">
         <v>68</v>
       </c>
@@ -1012,18 +1067,18 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="8"/>
+      <c r="I4" s="9"/>
       <c r="L4" t="s">
         <v>61</v>
       </c>
@@ -1038,18 +1093,18 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="8"/>
+      <c r="I5" s="9"/>
       <c r="L5" t="s">
         <v>62</v>
       </c>
@@ -1064,18 +1119,18 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="I6" s="8"/>
+      <c r="I6" s="9"/>
       <c r="L6" t="s">
         <v>63</v>
       </c>
@@ -1090,22 +1145,22 @@
       <c r="C7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8" t="s">
+      <c r="D7" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8" t="s">
+      <c r="E7" s="9"/>
+      <c r="F7" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="8" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8" t="s">
+      <c r="I7" s="9"/>
+      <c r="J7" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="K7" s="8"/>
+      <c r="K7" s="9"/>
       <c r="L7" s="10" t="s">
         <v>64</v>
       </c>
@@ -1114,44 +1169,44 @@
       <c r="A8" s="5"/>
       <c r="B8" s="6"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="8" t="s">
+      <c r="D8" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8" t="s">
+      <c r="E8" s="9"/>
+      <c r="F8" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="8" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="8" t="s">
+      <c r="I8" s="9"/>
+      <c r="J8" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="K8" s="8"/>
+      <c r="K8" s="9"/>
       <c r="L8" s="10"/>
     </row>
     <row r="9" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5"/>
       <c r="B9" s="6"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="8" t="s">
+      <c r="D9" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8" t="s">
+      <c r="E9" s="9"/>
+      <c r="F9" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="8" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8" t="s">
+      <c r="I9" s="9"/>
+      <c r="J9" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="K9" s="8"/>
+      <c r="K9" s="9"/>
       <c r="L9" s="10"/>
     </row>
     <row r="10" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1189,6 +1244,22 @@
     </row>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="D1:K1"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="H3:K3"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="H6:I6"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="F7:G7"/>
+    <mergeCell ref="H7:I7"/>
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="L7:L9"/>
     <mergeCell ref="J9:K9"/>
@@ -1199,22 +1270,6 @@
     <mergeCell ref="D8:E8"/>
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="H8:I8"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="H6:I6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="F7:G7"/>
-    <mergeCell ref="H7:I7"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="D1:K1"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="D3:G3"/>
-    <mergeCell ref="H3:K3"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1225,7 +1280,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:P17"/>
+      <selection activeCell="D3" sqref="D3:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1246,16 +1301,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1270,12 +1325,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -1290,22 +1345,22 @@
       <c r="C3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8" t="s">
+      <c r="E3" s="9"/>
+      <c r="F3" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8" t="s">
+      <c r="G3" s="9"/>
+      <c r="H3" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8" t="s">
+      <c r="I3" s="9"/>
+      <c r="J3" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="8"/>
+      <c r="K3" s="9"/>
       <c r="L3" t="s">
         <v>85</v>
       </c>
@@ -1320,22 +1375,22 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8" t="s">
+      <c r="E4" s="9"/>
+      <c r="F4" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="9" t="s">
         <v>88</v>
       </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="8" t="s">
+      <c r="I4" s="9"/>
+      <c r="J4" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K4" s="8"/>
+      <c r="K4" s="9"/>
       <c r="L4" t="s">
         <v>90</v>
       </c>
@@ -1350,22 +1405,22 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="8" t="s">
+      <c r="D5" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="9"/>
+      <c r="F5" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8" t="s">
+      <c r="I5" s="9"/>
+      <c r="J5" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="K5" s="8"/>
+      <c r="K5" s="9"/>
       <c r="L5" t="s">
         <v>95</v>
       </c>
@@ -1380,14 +1435,14 @@
       <c r="C6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8" t="s">
+      <c r="E6" s="9"/>
+      <c r="F6" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="9"/>
       <c r="L6" t="s">
         <v>98</v>
       </c>
@@ -1486,22 +1541,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="H4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
     <mergeCell ref="D1:K1"/>
     <mergeCell ref="D2:G2"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="H3:I3"/>
     <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="H4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1512,7 +1567,7 @@
   <dimension ref="A1:L4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:G3"/>
+      <selection activeCell="A2" sqref="A2:C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1532,16 +1587,16 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
       <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
@@ -1556,12 +1611,12 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
       <c r="L2" t="s">
         <v>11</v>
       </c>
@@ -1576,18 +1631,18 @@
       <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
-      <c r="H3" s="9" t="s">
+      <c r="E3" s="11"/>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="9"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="9"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
       <c r="L3" t="s">
         <v>13</v>
       </c>
@@ -1602,12 +1657,12 @@
       <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
       <c r="L4" t="s">
         <v>16</v>
       </c>
@@ -1626,31 +1681,36 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection sqref="A1:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="47.85546875" style="3" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1688,7 +1748,6 @@
         <v>33</v>
       </c>
       <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
@@ -1698,7 +1757,6 @@
         <v>107</v>
       </c>
       <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
@@ -1708,7 +1766,6 @@
         <v>108</v>
       </c>
       <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
@@ -1718,25 +1775,24 @@
         <v>109</v>
       </c>
       <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="E7" s="11" t="s">
+      <c r="E7" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="F7" s="11" t="s">
+      <c r="F7" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1884,8 +1940,208 @@
       <c r="E15" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="3" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>133</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E16" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>4</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19">
+        <v>8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20">
+        <v>8</v>
+      </c>
+      <c r="C20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21">
+        <v>4</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F22" s="8" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23">
+        <v>4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24">
+        <v>8</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E24" s="12">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="F24" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25" t="s">
+        <v>148</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E25" t="s">
+        <v>149</v>
+      </c>
+      <c r="F25" s="3" t="s">
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>